<commit_message>
added §§ and _si_
</commit_message>
<xml_diff>
--- a/examples/glossaries.xlsx
+++ b/examples/glossaries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Dev\ex2bib\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B8F6C1-3734-4934-AAB3-FAE0A3C33B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B5054D-D3B6-4F33-B256-45C234E465DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18285" yWindow="0" windowWidth="18750" windowHeight="15585" activeTab="1" xr2:uid="{26729782-A427-4FF2-A19B-DE9A1262909F}"/>
   </bookViews>
@@ -99,9 +99,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>\ensuremath{v}</t>
-  </si>
-  <si>
     <t>velocity</t>
   </si>
   <si>
@@ -111,31 +108,34 @@
     <t>x</t>
   </si>
   <si>
-    <t>\si{meter\per\second}</t>
-  </si>
-  <si>
-    <t>\si{m}</t>
-  </si>
-  <si>
-    <t>\ensuremath{x}</t>
-  </si>
-  <si>
     <t>position</t>
   </si>
   <si>
     <t>alpha</t>
   </si>
   <si>
-    <t>\si{\radian\per\second\squared}</t>
-  </si>
-  <si>
-    <t>\ensuremath{\alpha}</t>
-  </si>
-  <si>
     <t>angular acceleration</t>
   </si>
   <si>
     <t>greek</t>
+  </si>
+  <si>
+    <t>_si_metre\per\second</t>
+  </si>
+  <si>
+    <t>_si_m</t>
+  </si>
+  <si>
+    <t>_si_\radian\per\second\squared</t>
+  </si>
+  <si>
+    <t>$$v</t>
+  </si>
+  <si>
+    <t>$$x</t>
+  </si>
+  <si>
+    <t>$$\alpha</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,16 +608,16 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -625,19 +625,19 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -645,19 +645,19 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>